<commit_message>
sheet and loop update
</commit_message>
<xml_diff>
--- a/scientists.xlsx
+++ b/scientists.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="67">
   <si>
     <t>Cientista</t>
   </si>
@@ -98,10 +98,121 @@
     <t>Max Planck</t>
   </si>
   <si>
-    <t>Cientista Origem</t>
-  </si>
-  <si>
-    <t>Cientista Destino</t>
+    <t>Isaac Newton</t>
+  </si>
+  <si>
+    <t>John Freind</t>
+  </si>
+  <si>
+    <t>John Kiel</t>
+  </si>
+  <si>
+    <t>Robert Boyle</t>
+  </si>
+  <si>
+    <t>Daniel Bernoulli</t>
+  </si>
+  <si>
+    <t>John Herapath</t>
+  </si>
+  <si>
+    <t>John James Waterson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Antoine Lavoisier </t>
+  </si>
+  <si>
+    <t>John Dalton</t>
+  </si>
+  <si>
+    <t>Joseph Priestley</t>
+  </si>
+  <si>
+    <t>Charles Blagden</t>
+  </si>
+  <si>
+    <t>Henry Cavendish</t>
+  </si>
+  <si>
+    <t>William Henry</t>
+  </si>
+  <si>
+    <t>Joseph Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">André-Marie Ampère </t>
+  </si>
+  <si>
+    <t>Michael Faraday</t>
+  </si>
+  <si>
+    <t>Heirich Hertz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amedeo Avogadro </t>
+  </si>
+  <si>
+    <t>Jacob Berzellius</t>
+  </si>
+  <si>
+    <t>Henry Becquerel</t>
+  </si>
+  <si>
+    <t>James Chadwick</t>
+  </si>
+  <si>
+    <t>Cientista_Origem</t>
+  </si>
+  <si>
+    <t>Cientista_Destino</t>
+  </si>
+  <si>
+    <t>Seculo_Interacao</t>
+  </si>
+  <si>
+    <t>Heinrich Hertz</t>
+  </si>
+  <si>
+    <t>Humphry Davy</t>
+  </si>
+  <si>
+    <t>William Wollaston</t>
+  </si>
+  <si>
+    <t>Louis J. Gay-Lussac</t>
+  </si>
+  <si>
+    <t>Amedeo Avogadro</t>
+  </si>
+  <si>
+    <t>Claude Louis Berthollet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jacob Berzellius </t>
+  </si>
+  <si>
+    <t>Giovanni Cantoni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robert Brown </t>
+  </si>
+  <si>
+    <t>Bodoszewski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max Planck </t>
+  </si>
+  <si>
+    <t>Marie Curie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daniel Bernoulli </t>
+  </si>
+  <si>
+    <t>Antoine Lavoisier</t>
+  </si>
+  <si>
+    <t>André-Marie Àmpere</t>
   </si>
 </sst>
 </file>
@@ -514,6 +625,111 @@
         <v>27</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -531,14 +747,18 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="18.5"/>
     <col customWidth="1" min="2" max="2" width="20.25"/>
+    <col customWidth="1" min="3" max="3" width="15.38"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2">
@@ -548,6 +768,9 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -556,6 +779,9 @@
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
@@ -564,6 +790,9 @@
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
@@ -572,6 +801,9 @@
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
@@ -580,6 +812,9 @@
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
@@ -588,6 +823,9 @@
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="C7" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
@@ -596,6 +834,9 @@
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
@@ -604,6 +845,9 @@
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
@@ -612,6 +856,9 @@
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="C10" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
@@ -620,6 +867,9 @@
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C11" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
@@ -628,6 +878,9 @@
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="C12" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
@@ -636,6 +889,9 @@
       <c r="B13" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C13" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
@@ -644,6 +900,9 @@
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C14" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
@@ -652,6 +911,9 @@
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C15" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
@@ -660,6 +922,9 @@
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C16" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
@@ -668,6 +933,9 @@
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C17" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
@@ -676,6 +944,9 @@
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="C18" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
@@ -684,6 +955,9 @@
       <c r="B19" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C19" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
@@ -692,6 +966,9 @@
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C20" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
@@ -700,6 +977,9 @@
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="C21" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
@@ -708,6 +988,9 @@
       <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C22" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -716,6 +999,9 @@
       <c r="B23" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="C23" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
@@ -724,6 +1010,9 @@
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C24" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -732,6 +1021,9 @@
       <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C25" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
@@ -740,6 +1032,9 @@
       <c r="B26" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C26" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
@@ -748,6 +1043,9 @@
       <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="C27" s="2">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
@@ -755,6 +1053,339 @@
       </c>
       <c r="B28" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="C28" s="2">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="2">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C46" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C53" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C57" s="2">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C58" s="2">
+        <v>18.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>